<commit_message>
Updated metadata template to comply with new metadata including the Schulman Shift.
</commit_message>
<xml_diff>
--- a/TRIAD-metadata-template-2020-09-14.xlsx
+++ b/TRIAD-metadata-template-2020-09-14.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">Your name</t>
   </si>
@@ -34,12 +34,12 @@
     <t xml:space="preserve">Sample Date (YYYY-MM-DD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample Year</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sample Year Growth</t>
   </si>
   <si>
+    <t xml:space="preserve">Schulman Shift</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scan resolution (DPI)</t>
   </si>
   <si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">Sample ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Sample height (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample azimuth ()</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample note</t>
   </si>
   <si>
@@ -86,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">BigChill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">This tree was chilled at 1 and 2 m aboveground during the 2018 growing season.</t>
@@ -209,10 +218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -221,9 +230,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="21.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="21.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,25 +286,31 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>44047</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>19</v>
+      <c r="E2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>3600</v>
@@ -307,10 +324,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>5</v>
@@ -318,14 +335,20 @@
       <c r="M2" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>22</v>
+      <c r="N2" s="0" t="n">
+        <v>1.5</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>